<commit_message>
Support header / footer on excel
</commit_message>
<xml_diff>
--- a/src/main/webapp/WEB-INF/data/excel/R172_STA_TS-Brainstorming_v2.15.xlsx
+++ b/src/main/webapp/WEB-INF/data/excel/R172_STA_TS-Brainstorming_v2.15.xlsx
@@ -1,27 +1,27 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="25601"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="25928"/>
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl.localhost\Ubuntu-20.04\home\eomar\git\TrickService\src\main\webapp\WEB-INF\data\excel\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl.localhost\Ubuntu-22.04\home\eomar\git\trickservice\src\main\webapp\WEB-INF\data\excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:201_{46E487D1-667B-45BF-BB96-3342E4EF0137}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:201_{D4AEC398-E706-4DAA-BAA8-5D760D1B30F2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4005" yWindow="1290" windowWidth="21600" windowHeight="11295" tabRatio="733" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28920" yWindow="1005" windowWidth="29040" windowHeight="15720" tabRatio="733" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Hist" sheetId="3" r:id="rId1"/>
-    <sheet name="Threats" sheetId="38" r:id="rId2"/>
-    <sheet name="Vulnerabilities" sheetId="40" r:id="rId3"/>
-    <sheet name="Risks" sheetId="39" r:id="rId4"/>
-    <sheet name="Structure" sheetId="17" r:id="rId5"/>
-    <sheet name="Guide" sheetId="37" r:id="rId6"/>
+    <sheet name="Structure" sheetId="17" r:id="rId2"/>
+    <sheet name="Guide" sheetId="37" r:id="rId3"/>
+    <sheet name="Threats" sheetId="38" r:id="rId4"/>
+    <sheet name="Vulnerabilities" sheetId="40" r:id="rId5"/>
+    <sheet name="Risks" sheetId="39" r:id="rId6"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm.Print_Area" localSheetId="5">Guide!$A$1:$E$35</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="2">Guide!$A$1:$E$35</definedName>
     <definedName name="_xlnm.Print_Area" localSheetId="0">Hist!$A$1:$D$18</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
@@ -1097,6 +1097,27 @@
     <xf numFmtId="0" fontId="14" fillId="0" borderId="16" xfId="5" applyBorder="1">
       <alignment horizontal="left" vertical="top" wrapText="1" indent="1"/>
     </xf>
+    <xf numFmtId="0" fontId="18" fillId="3" borderId="1" xfId="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="4" borderId="1" xfId="2">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="5" borderId="1" xfId="3">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="7" borderId="8" xfId="4" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="13" xfId="5" applyBorder="1">
+      <alignment horizontal="left" vertical="top" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="14" xfId="5" applyBorder="1">
+      <alignment horizontal="left" vertical="top" wrapText="1" indent="1"/>
+    </xf>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="17" xfId="5" applyBorder="1">
       <alignment horizontal="left" vertical="top" wrapText="1" indent="1"/>
     </xf>
@@ -1106,12 +1127,6 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="5" borderId="1" xfId="3">
-      <alignment horizontal="left" vertical="center" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="165" fontId="14" fillId="0" borderId="15" xfId="8" applyBorder="1">
       <alignment horizontal="left" vertical="top" indent="1"/>
     </xf>
@@ -1120,21 +1135,6 @@
     </xf>
     <xf numFmtId="0" fontId="13" fillId="7" borderId="5" xfId="4" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="3" borderId="1" xfId="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="4" borderId="1" xfId="2">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="7" borderId="8" xfId="4" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="13" xfId="5" applyBorder="1">
-      <alignment horizontal="left" vertical="top" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="14" xfId="5" applyBorder="1">
-      <alignment horizontal="left" vertical="top" wrapText="1" indent="1"/>
     </xf>
     <xf numFmtId="0" fontId="18" fillId="3" borderId="2" xfId="1" applyBorder="1">
       <alignment horizontal="center" vertical="center"/>
@@ -3181,6 +3181,33 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table3" displayName="Table3" ref="A1:D6" totalsRowShown="0" headerRowDxfId="3" headerRowCellStyle="Cell-Normal" dataCellStyle="Cell-Normal">
+  <autoFilter ref="A1:D6" xr:uid="{00000000-0009-0000-0100-000003000000}"/>
+  <tableColumns count="4">
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Tab name" dataCellStyle="Heading 4"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Contents" dataDxfId="2" dataCellStyle="Cell-Normal"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="Comments" dataDxfId="1" dataCellStyle="Cell-Normal"/>
+    <tableColumn id="4" xr3:uid="{1B8FDF6E-4960-4789-98B3-58D222A2D1F8}" name="Void" dataDxfId="0" dataCellStyle="Cell-Normal"/>
+  </tableColumns>
+  <tableStyleInfo name="Table_B" showFirstColumn="1" showLastColumn="0" showRowStripes="0" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{EB3165EA-BCD9-474A-8AA5-F5F7C967F3E7}" name="Table4" displayName="Table4" ref="D1:E35" totalsRowShown="0" headerRowCellStyle="Cell-Normal" dataCellStyle="Cell-Normal">
+  <autoFilter ref="D1:E35" xr:uid="{844509D7-165E-41F0-8A6E-A5CE2C2144EA}"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="D2:E35">
+    <sortCondition ref="D2:D35"/>
+  </sortState>
+  <tableColumns count="2">
+    <tableColumn id="1" xr3:uid="{AB32D27C-F241-418A-857E-BA1A154A4171}" name="Type" dataCellStyle="Cell-Normal"/>
+    <tableColumn id="2" xr3:uid="{3E8A8340-04C3-4678-9525-578C1CEA4534}" name="Description" dataCellStyle="Cell-Normal"/>
+  </tableColumns>
+  <tableStyleInfo name="Table_B" showFirstColumn="1" showLastColumn="0" showRowStripes="0" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{C1CEF948-26B0-4FBA-8C1E-EFD91A6E508D}" name="ThreatTable" displayName="ThreatTable" ref="A1:G2" totalsRowShown="0" headerRowCellStyle="Cell-wrapped" dataCellStyle="Cell-wrapped">
   <autoFilter ref="A1:G2" xr:uid="{00000000-0009-0000-0100-000003000000}"/>
   <tableColumns count="7">
@@ -3196,7 +3223,7 @@
 </table>
 </file>
 
-<file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{38A68276-F885-48BE-AEF4-B56204AC8375}" name="VulTable" displayName="VulTable" ref="A1:F2" totalsRowShown="0" headerRowCellStyle="Cell-wrapped" dataCellStyle="Cell-wrapped">
   <autoFilter ref="A1:F2" xr:uid="{00000000-0009-0000-0100-000003000000}"/>
   <tableColumns count="6">
@@ -3211,7 +3238,7 @@
 </table>
 </file>
 
-<file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{9350F8C0-815D-4FF5-9D88-9550F8F4A1A6}" name="RiskTable" displayName="RiskTable" ref="A1:F2" totalsRowShown="0" headerRowDxfId="11" headerRowCellStyle="Cell-wrapped" dataCellStyle="Cell-wrapped">
   <autoFilter ref="A1:F2" xr:uid="{00000000-0009-0000-0100-000003000000}"/>
   <tableColumns count="6">
@@ -3221,33 +3248,6 @@
     <tableColumn id="4" xr3:uid="{0402EB88-9CBA-4DF2-BF51-F34DF4B9CD1E}" name="Owner" dataDxfId="9" dataCellStyle="Cell-wrapped"/>
     <tableColumn id="5" xr3:uid="{A1F3E8FF-91E2-410D-A89A-9E3AB22EA76A}" name="Comment" dataDxfId="8" dataCellStyle="Cell-wrapped"/>
     <tableColumn id="6" xr3:uid="{1512FC01-983A-4692-9EC3-73C044480E39}" name="Hidden Comment" dataDxfId="7" dataCellStyle="Cell-wrapped"/>
-  </tableColumns>
-  <tableStyleInfo name="Table_B" showFirstColumn="1" showLastColumn="0" showRowStripes="0" showColumnStripes="0"/>
-</table>
-</file>
-
-<file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table3" displayName="Table3" ref="A1:D6" totalsRowShown="0" headerRowDxfId="3" headerRowCellStyle="Cell-Normal" dataCellStyle="Cell-Normal">
-  <autoFilter ref="A1:D6" xr:uid="{00000000-0009-0000-0100-000003000000}"/>
-  <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Tab name" dataCellStyle="Heading 4"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Contents" dataDxfId="2" dataCellStyle="Cell-Normal"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="Comments" dataDxfId="1" dataCellStyle="Cell-Normal"/>
-    <tableColumn id="4" xr3:uid="{1B8FDF6E-4960-4789-98B3-58D222A2D1F8}" name="Void" dataDxfId="0" dataCellStyle="Cell-Normal"/>
-  </tableColumns>
-  <tableStyleInfo name="Table_B" showFirstColumn="1" showLastColumn="0" showRowStripes="0" showColumnStripes="0"/>
-</table>
-</file>
-
-<file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{EB3165EA-BCD9-474A-8AA5-F5F7C967F3E7}" name="Table4" displayName="Table4" ref="D1:E35" totalsRowShown="0" headerRowCellStyle="Cell-Normal" dataCellStyle="Cell-Normal">
-  <autoFilter ref="D1:E35" xr:uid="{844509D7-165E-41F0-8A6E-A5CE2C2144EA}"/>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="D2:E35">
-    <sortCondition ref="D2:D35"/>
-  </sortState>
-  <tableColumns count="2">
-    <tableColumn id="1" xr3:uid="{AB32D27C-F241-418A-857E-BA1A154A4171}" name="Type" dataCellStyle="Cell-Normal"/>
-    <tableColumn id="2" xr3:uid="{3E8A8340-04C3-4678-9525-578C1CEA4534}" name="Description" dataCellStyle="Cell-Normal"/>
   </tableColumns>
   <tableStyleInfo name="Table_B" showFirstColumn="1" showLastColumn="0" showRowStripes="0" showColumnStripes="0"/>
 </table>
@@ -3461,7 +3461,7 @@
   </sheetPr>
   <dimension ref="A1:G21"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="110" workbookViewId="0">
+    <sheetView zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="110" workbookViewId="0">
       <selection activeCell="C5" sqref="C5:D5"/>
     </sheetView>
   </sheetViews>
@@ -3475,26 +3475,26 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="22.5" x14ac:dyDescent="0.2">
-      <c r="A1" s="43" t="s">
+      <c r="A1" s="35" t="s">
         <v>128</v>
       </c>
-      <c r="B1" s="43"/>
-      <c r="C1" s="43"/>
-      <c r="D1" s="43"/>
+      <c r="B1" s="35"/>
+      <c r="C1" s="35"/>
+      <c r="D1" s="35"/>
     </row>
     <row r="2" spans="1:7" s="2" customFormat="1" ht="23.25" x14ac:dyDescent="0.2">
-      <c r="A2" s="44" t="s">
+      <c r="A2" s="36" t="s">
         <v>129</v>
       </c>
-      <c r="B2" s="44"/>
-      <c r="C2" s="44"/>
-      <c r="D2" s="44"/>
+      <c r="B2" s="36"/>
+      <c r="C2" s="36"/>
+      <c r="D2" s="36"/>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A3" s="39"/>
-      <c r="B3" s="39"/>
-      <c r="C3" s="39"/>
-      <c r="D3" s="39"/>
+      <c r="A3" s="37"/>
+      <c r="B3" s="37"/>
+      <c r="C3" s="37"/>
+      <c r="D3" s="37"/>
       <c r="G3" s="7"/>
     </row>
     <row r="4" spans="1:7" ht="15.75" x14ac:dyDescent="0.2">
@@ -3506,14 +3506,14 @@
       <c r="D4" s="38"/>
     </row>
     <row r="5" spans="1:7" s="3" customFormat="1" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="A5" s="45" t="s">
+      <c r="A5" s="39" t="s">
         <v>22</v>
       </c>
-      <c r="B5" s="45"/>
-      <c r="C5" s="46" t="s">
+      <c r="B5" s="39"/>
+      <c r="C5" s="40" t="s">
         <v>137</v>
       </c>
-      <c r="D5" s="47"/>
+      <c r="D5" s="41"/>
     </row>
     <row r="6" spans="1:7" s="3" customFormat="1" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A6" s="32" t="s">
@@ -3553,29 +3553,29 @@
         <v>23</v>
       </c>
       <c r="B9" s="32"/>
-      <c r="C9" s="40">
+      <c r="C9" s="45">
         <v>44827</v>
       </c>
-      <c r="D9" s="41"/>
+      <c r="D9" s="46"/>
       <c r="F9" s="12" t="s">
         <v>48</v>
       </c>
     </row>
     <row r="10" spans="1:7" s="3" customFormat="1" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="A10" s="42" t="s">
+      <c r="A10" s="47" t="s">
         <v>1</v>
       </c>
-      <c r="B10" s="42"/>
-      <c r="C10" s="35" t="s">
+      <c r="B10" s="47"/>
+      <c r="C10" s="42" t="s">
         <v>20</v>
       </c>
-      <c r="D10" s="36"/>
+      <c r="D10" s="43"/>
     </row>
     <row r="11" spans="1:7" s="3" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A11" s="37"/>
-      <c r="B11" s="37"/>
-      <c r="C11" s="37"/>
-      <c r="D11" s="37"/>
+      <c r="A11" s="44"/>
+      <c r="B11" s="44"/>
+      <c r="C11" s="44"/>
+      <c r="D11" s="44"/>
     </row>
     <row r="12" spans="1:7" ht="15.75" x14ac:dyDescent="0.2">
       <c r="A12" s="38" t="s">
@@ -3615,10 +3615,10 @@
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A15" s="39"/>
-      <c r="B15" s="39"/>
-      <c r="C15" s="39"/>
-      <c r="D15" s="39"/>
+      <c r="A15" s="37"/>
+      <c r="B15" s="37"/>
+      <c r="C15" s="37"/>
+      <c r="D15" s="37"/>
     </row>
     <row r="16" spans="1:7" ht="15.75" x14ac:dyDescent="0.2">
       <c r="A16" s="38" t="s">
@@ -3674,6 +3674,16 @@
     </row>
   </sheetData>
   <mergeCells count="20">
+    <mergeCell ref="A8:B8"/>
+    <mergeCell ref="C8:D8"/>
+    <mergeCell ref="C10:D10"/>
+    <mergeCell ref="A11:D11"/>
+    <mergeCell ref="A16:D16"/>
+    <mergeCell ref="A12:D12"/>
+    <mergeCell ref="A15:D15"/>
+    <mergeCell ref="A9:B9"/>
+    <mergeCell ref="C9:D9"/>
+    <mergeCell ref="A10:B10"/>
     <mergeCell ref="A6:B6"/>
     <mergeCell ref="C6:D6"/>
     <mergeCell ref="A7:B7"/>
@@ -3684,16 +3694,6 @@
     <mergeCell ref="A4:D4"/>
     <mergeCell ref="A5:B5"/>
     <mergeCell ref="C5:D5"/>
-    <mergeCell ref="A8:B8"/>
-    <mergeCell ref="C8:D8"/>
-    <mergeCell ref="C10:D10"/>
-    <mergeCell ref="A11:D11"/>
-    <mergeCell ref="A16:D16"/>
-    <mergeCell ref="A12:D12"/>
-    <mergeCell ref="A15:D15"/>
-    <mergeCell ref="A9:B9"/>
-    <mergeCell ref="C9:D9"/>
-    <mergeCell ref="A10:B10"/>
   </mergeCells>
   <phoneticPr fontId="8" type="noConversion"/>
   <printOptions horizontalCentered="1"/>
@@ -3715,239 +3715,6 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6D9F6A2C-208A-4360-A537-CE38C4E0741D}">
-  <sheetPr codeName="Sheet4"/>
-  <dimension ref="A1:G2"/>
-  <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:B2"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="9.1640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
-  <cols>
-    <col min="1" max="1" width="6.5" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10.33203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="13.5" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="13.1640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="11.1640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="14.5" style="1" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="23" style="1" bestFit="1" customWidth="1"/>
-    <col min="8" max="16384" width="9.1640625" style="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A1" s="30" t="s">
-        <v>132</v>
-      </c>
-      <c r="B1" s="30" t="s">
-        <v>5</v>
-      </c>
-      <c r="C1" s="30" t="s">
-        <v>133</v>
-      </c>
-      <c r="D1" s="30" t="s">
-        <v>134</v>
-      </c>
-      <c r="E1" s="29" t="s">
-        <v>7</v>
-      </c>
-      <c r="F1" s="29" t="s">
-        <v>135</v>
-      </c>
-      <c r="G1" s="29" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A2" s="7"/>
-      <c r="B2" s="7"/>
-      <c r="C2" s="29"/>
-      <c r="D2" s="29"/>
-      <c r="E2" s="29"/>
-      <c r="F2" s="29"/>
-      <c r="G2" s="29"/>
-    </row>
-  </sheetData>
-  <conditionalFormatting sqref="B2">
-    <cfRule type="cellIs" dxfId="29" priority="1" stopIfTrue="1" operator="equal">
-      <formula>"Policy"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="28" priority="2" stopIfTrue="1" operator="equal">
-      <formula>"Procedure"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="27" priority="3" stopIfTrue="1" operator="equal">
-      <formula>"Standard"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <pageMargins left="0.19685039370078741" right="0.19685039370078741" top="0.94488188976377963" bottom="0.74803149606299213" header="0.31496062992125984" footer="0.31496062992125984"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
-  <headerFooter>
-    <oddHeader>&amp;L&amp;"Corbel,Regular"&amp;G&amp;R&amp;K08+000 Activity:&amp;K01+000ISMS&amp;K08+000
- Title:&amp;K01+000 TS-Export
-&amp;K08+000 Classification:&amp;K01+000 Restricted</oddHeader>
-    <oddFooter>&amp;L&amp;"Corbel,Regular"&amp;F&amp;C&amp;"Corbel,Regular"&amp;D - &amp;T&amp;R
-&amp;"Corbel,Regular"&amp;A - &amp;P/&amp;N</oddFooter>
-  </headerFooter>
-  <legacyDrawingHF r:id="rId2"/>
-  <tableParts count="1">
-    <tablePart r:id="rId3"/>
-  </tableParts>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0D00A1E2-2C67-4E04-ABA3-40DC628DF38D}">
-  <sheetPr codeName="Sheet7"/>
-  <dimension ref="A1:F2"/>
-  <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:B2"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="9.1640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
-  <cols>
-    <col min="1" max="1" width="6.5" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="17" style="1" customWidth="1"/>
-    <col min="3" max="3" width="10.1640625" style="1" customWidth="1"/>
-    <col min="4" max="4" width="11.1640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="14.5" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="23" style="1" bestFit="1" customWidth="1"/>
-    <col min="7" max="16384" width="9.1640625" style="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A1" s="30" t="s">
-        <v>132</v>
-      </c>
-      <c r="B1" s="30" t="s">
-        <v>5</v>
-      </c>
-      <c r="C1" s="30" t="s">
-        <v>134</v>
-      </c>
-      <c r="D1" s="30" t="s">
-        <v>7</v>
-      </c>
-      <c r="E1" s="29" t="s">
-        <v>135</v>
-      </c>
-      <c r="F1" s="29" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A2" s="31"/>
-      <c r="B2" s="31"/>
-      <c r="C2" s="29"/>
-      <c r="D2" s="29"/>
-      <c r="E2" s="29"/>
-      <c r="F2" s="29"/>
-    </row>
-  </sheetData>
-  <conditionalFormatting sqref="B2">
-    <cfRule type="cellIs" dxfId="21" priority="1" stopIfTrue="1" operator="equal">
-      <formula>"Policy"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="20" priority="2" stopIfTrue="1" operator="equal">
-      <formula>"Procedure"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="19" priority="3" stopIfTrue="1" operator="equal">
-      <formula>"Standard"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <pageMargins left="0.19685039370078741" right="0.19685039370078741" top="0.94488188976377963" bottom="0.74803149606299213" header="0.31496062992125984" footer="0.31496062992125984"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
-  <headerFooter>
-    <oddHeader>&amp;L&amp;"Corbel,Regular"&amp;G&amp;R&amp;K08+000 Activity:&amp;K01+000ISMS&amp;K08+000
- Title:&amp;K01+000 TS-Export
-&amp;K08+000 Classification:&amp;K01+000 Restricted</oddHeader>
-    <oddFooter>&amp;L&amp;"Corbel,Regular"&amp;F&amp;C&amp;"Corbel,Regular"&amp;D - &amp;T&amp;R
-&amp;"Corbel,Regular"&amp;A - &amp;P/&amp;N</oddFooter>
-  </headerFooter>
-  <legacyDrawingHF r:id="rId2"/>
-  <tableParts count="1">
-    <tablePart r:id="rId3"/>
-  </tableParts>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{37A202E0-B862-4A14-99BA-66891FB3DD63}">
-  <sheetPr codeName="Sheet6"/>
-  <dimension ref="A1:F2"/>
-  <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="E20" sqref="E20"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="9.1640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
-  <cols>
-    <col min="1" max="1" width="11.33203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="15.83203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="19.83203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="17.1640625" style="1" customWidth="1"/>
-    <col min="5" max="5" width="21.33203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="33.5" style="1" bestFit="1" customWidth="1"/>
-    <col min="7" max="16384" width="9.1640625" style="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A1" s="28" t="s">
-        <v>132</v>
-      </c>
-      <c r="B1" s="28" t="s">
-        <v>5</v>
-      </c>
-      <c r="C1" s="28" t="s">
-        <v>134</v>
-      </c>
-      <c r="D1" s="28" t="s">
-        <v>7</v>
-      </c>
-      <c r="E1" s="28" t="s">
-        <v>135</v>
-      </c>
-      <c r="F1" s="28" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A2" s="7"/>
-      <c r="B2" s="7"/>
-      <c r="C2" s="29"/>
-      <c r="D2" s="29"/>
-      <c r="E2" s="29"/>
-      <c r="F2" s="29"/>
-    </row>
-  </sheetData>
-  <conditionalFormatting sqref="B2">
-    <cfRule type="cellIs" dxfId="14" priority="1" stopIfTrue="1" operator="equal">
-      <formula>"Policy"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="13" priority="2" stopIfTrue="1" operator="equal">
-      <formula>"Procedure"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="12" priority="3" stopIfTrue="1" operator="equal">
-      <formula>"Standard"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <pageMargins left="0.19685039370078741" right="0.19685039370078741" top="0.94488188976377963" bottom="0.74803149606299213" header="0.31496062992125984" footer="0.31496062992125984"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
-  <headerFooter>
-    <oddHeader>&amp;L&amp;"Corbel,Regular"&amp;G&amp;R&amp;K08+000 Activity:&amp;K01+000ISMS&amp;K08+000
- Title:&amp;K01+000 TS-Export
-&amp;K08+000 Classification:&amp;K01+000 Restricted</oddHeader>
-    <oddFooter>&amp;L&amp;"Corbel,Regular"&amp;F&amp;C&amp;"Corbel,Regular"&amp;D - &amp;T&amp;R
-&amp;"Corbel,Regular"&amp;A - &amp;P/&amp;N</oddFooter>
-  </headerFooter>
-  <legacyDrawingHF r:id="rId2"/>
-  <tableParts count="1">
-    <tablePart r:id="rId3"/>
-  </tableParts>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <sheetPr codeName="Sheet3"/>
   <dimension ref="A1:D6"/>
@@ -4073,7 +3840,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BD4946C6-2E76-46C4-A2AB-3FEEF6D7E257}">
   <sheetPr codeName="Sheet5"/>
   <dimension ref="A1:E35"/>
@@ -4474,4 +4241,237 @@
     <tablePart r:id="rId3"/>
   </tableParts>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6D9F6A2C-208A-4360-A537-CE38C4E0741D}">
+  <sheetPr codeName="Sheet4"/>
+  <dimension ref="A1:G2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:B2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9.1640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="6.5" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.33203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.5" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.1640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.1640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="14.5" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="23" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="16384" width="9.1640625" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A1" s="30" t="s">
+        <v>132</v>
+      </c>
+      <c r="B1" s="30" t="s">
+        <v>5</v>
+      </c>
+      <c r="C1" s="30" t="s">
+        <v>133</v>
+      </c>
+      <c r="D1" s="30" t="s">
+        <v>134</v>
+      </c>
+      <c r="E1" s="29" t="s">
+        <v>7</v>
+      </c>
+      <c r="F1" s="29" t="s">
+        <v>135</v>
+      </c>
+      <c r="G1" s="29" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A2" s="7"/>
+      <c r="B2" s="7"/>
+      <c r="C2" s="29"/>
+      <c r="D2" s="29"/>
+      <c r="E2" s="29"/>
+      <c r="F2" s="29"/>
+      <c r="G2" s="29"/>
+    </row>
+  </sheetData>
+  <conditionalFormatting sqref="B2">
+    <cfRule type="cellIs" dxfId="29" priority="1" stopIfTrue="1" operator="equal">
+      <formula>"Policy"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="28" priority="2" stopIfTrue="1" operator="equal">
+      <formula>"Procedure"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="27" priority="3" stopIfTrue="1" operator="equal">
+      <formula>"Standard"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <pageMargins left="0.19685039370078741" right="0.19685039370078741" top="0.94488188976377963" bottom="0.74803149606299213" header="0.31496062992125984" footer="0.31496062992125984"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+  <headerFooter>
+    <oddHeader>&amp;L&amp;"Corbel,Regular"&amp;G&amp;R&amp;K08+000 Activity:&amp;K01+000ISMS&amp;K08+000
+ Title:&amp;K01+000 TS-Export
+&amp;K08+000 Classification:&amp;K01+000 Restricted</oddHeader>
+    <oddFooter>&amp;L&amp;"Corbel,Regular"&amp;F&amp;C&amp;"Corbel,Regular"&amp;D - &amp;T&amp;R
+&amp;"Corbel,Regular"&amp;A - &amp;P/&amp;N</oddFooter>
+  </headerFooter>
+  <legacyDrawingHF r:id="rId2"/>
+  <tableParts count="1">
+    <tablePart r:id="rId3"/>
+  </tableParts>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0D00A1E2-2C67-4E04-ABA3-40DC628DF38D}">
+  <sheetPr codeName="Sheet7"/>
+  <dimension ref="A1:F2"/>
+  <sheetViews>
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9.1640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="6.5" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="17" style="1" customWidth="1"/>
+    <col min="3" max="3" width="10.1640625" style="1" customWidth="1"/>
+    <col min="4" max="4" width="11.1640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14.5" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="23" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="16384" width="9.1640625" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A1" s="30" t="s">
+        <v>132</v>
+      </c>
+      <c r="B1" s="30" t="s">
+        <v>5</v>
+      </c>
+      <c r="C1" s="30" t="s">
+        <v>134</v>
+      </c>
+      <c r="D1" s="30" t="s">
+        <v>7</v>
+      </c>
+      <c r="E1" s="29" t="s">
+        <v>135</v>
+      </c>
+      <c r="F1" s="29" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A2" s="31"/>
+      <c r="B2" s="31"/>
+      <c r="C2" s="29"/>
+      <c r="D2" s="29"/>
+      <c r="E2" s="29"/>
+      <c r="F2" s="29"/>
+    </row>
+  </sheetData>
+  <conditionalFormatting sqref="B2">
+    <cfRule type="cellIs" dxfId="21" priority="1" stopIfTrue="1" operator="equal">
+      <formula>"Policy"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="20" priority="2" stopIfTrue="1" operator="equal">
+      <formula>"Procedure"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="19" priority="3" stopIfTrue="1" operator="equal">
+      <formula>"Standard"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <pageMargins left="0.19685039370078741" right="0.19685039370078741" top="0.94488188976377963" bottom="0.74803149606299213" header="0.31496062992125984" footer="0.31496062992125984"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+  <headerFooter>
+    <oddHeader>&amp;L&amp;"Corbel,Regular"&amp;G&amp;R&amp;K08+000 Activity:&amp;K01+000ISMS&amp;K08+000
+ Title:&amp;K01+000 TS-Export
+&amp;K08+000 Classification:&amp;K01+000 Restricted</oddHeader>
+    <oddFooter>&amp;L&amp;"Corbel,Regular"&amp;F&amp;C&amp;"Corbel,Regular"&amp;D - &amp;T&amp;R
+&amp;"Corbel,Regular"&amp;A - &amp;P/&amp;N</oddFooter>
+  </headerFooter>
+  <legacyDrawingHF r:id="rId2"/>
+  <tableParts count="1">
+    <tablePart r:id="rId3"/>
+  </tableParts>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{37A202E0-B862-4A14-99BA-66891FB3DD63}">
+  <sheetPr codeName="Sheet6"/>
+  <dimension ref="A1:F2"/>
+  <sheetViews>
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="E20" sqref="E20"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9.1640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="11.33203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.83203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="19.83203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="17.1640625" style="1" customWidth="1"/>
+    <col min="5" max="5" width="21.33203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="33.5" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="16384" width="9.1640625" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A1" s="28" t="s">
+        <v>132</v>
+      </c>
+      <c r="B1" s="28" t="s">
+        <v>5</v>
+      </c>
+      <c r="C1" s="28" t="s">
+        <v>134</v>
+      </c>
+      <c r="D1" s="28" t="s">
+        <v>7</v>
+      </c>
+      <c r="E1" s="28" t="s">
+        <v>135</v>
+      </c>
+      <c r="F1" s="28" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A2" s="7"/>
+      <c r="B2" s="7"/>
+      <c r="C2" s="29"/>
+      <c r="D2" s="29"/>
+      <c r="E2" s="29"/>
+      <c r="F2" s="29"/>
+    </row>
+  </sheetData>
+  <conditionalFormatting sqref="B2">
+    <cfRule type="cellIs" dxfId="14" priority="1" stopIfTrue="1" operator="equal">
+      <formula>"Policy"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="13" priority="2" stopIfTrue="1" operator="equal">
+      <formula>"Procedure"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="12" priority="3" stopIfTrue="1" operator="equal">
+      <formula>"Standard"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <pageMargins left="0.19685039370078741" right="0.19685039370078741" top="0.94488188976377963" bottom="0.74803149606299213" header="0.31496062992125984" footer="0.31496062992125984"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+  <headerFooter>
+    <oddHeader>&amp;L&amp;"Corbel,Regular"&amp;G&amp;R&amp;K08+000 Activity:&amp;K01+000ISMS&amp;K08+000
+ Title:&amp;K01+000 TS-Export
+&amp;K08+000 Classification:&amp;K01+000 Restricted</oddHeader>
+    <oddFooter>&amp;L&amp;"Corbel,Regular"&amp;F&amp;C&amp;"Corbel,Regular"&amp;D - &amp;T&amp;R
+&amp;"Corbel,Regular"&amp;A - &amp;P/&amp;N</oddFooter>
+  </headerFooter>
+  <legacyDrawingHF r:id="rId2"/>
+  <tableParts count="1">
+    <tablePart r:id="rId3"/>
+  </tableParts>
+</worksheet>
 </file>
</xml_diff>